<commit_message>
Maj diagramme de classes
</commit_message>
<xml_diff>
--- a/modelisator/Gestion de projet/2015_06_10 [Modelisator] Step 4/Dictionnaire de données organisé.xlsx
+++ b/modelisator/Gestion de projet/2015_06_10 [Modelisator] Step 4/Dictionnaire de données organisé.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Utilisateur</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Contexte liste P</t>
   </si>
   <si>
-    <t>Objet seléctionné (P ou GP)</t>
-  </si>
-  <si>
     <t>Fenêtre d'authentification</t>
   </si>
   <si>
@@ -136,9 +133,6 @@
     <t>VUE</t>
   </si>
   <si>
-    <t>Feuille de calcul</t>
-  </si>
-  <si>
     <t>Historique</t>
   </si>
   <si>
@@ -149,6 +143,27 @@
   </si>
   <si>
     <t>Contexte</t>
+  </si>
+  <si>
+    <t>Sauvegarde</t>
+  </si>
+  <si>
+    <t>Sélectionné</t>
+  </si>
+  <si>
+    <t>Date sauvegarde</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>Nom fichier</t>
+  </si>
+  <si>
+    <t>import()</t>
+  </si>
+  <si>
+    <t>export()</t>
   </si>
 </sst>
 </file>
@@ -239,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -247,6 +262,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,22 +567,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H34"/>
+  <dimension ref="B1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
     <col min="3" max="3" width="3.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
     <col min="5" max="5" width="3.5703125" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" customWidth="1"/>
     <col min="7" max="7" width="3" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" customWidth="1"/>
     <col min="9" max="9" width="3.42578125" customWidth="1"/>
     <col min="10" max="10" width="9.140625" customWidth="1"/>
   </cols>
@@ -591,7 +607,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>5</v>
@@ -611,39 +627,46 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F5" s="3" t="s">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="H6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H7" s="3" t="s">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>19</v>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>10</v>
@@ -653,6 +676,9 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
@@ -661,111 +687,124 @@
       </c>
     </row>
     <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="D12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
         <v>39</v>
       </c>
     </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>20</v>
+      <c r="B16" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>